<commit_message>
Add Persian and Japanese translated texts
</commit_message>
<xml_diff>
--- a/documents/translations.xlsx
+++ b/documents/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\IdeaProjects\OTP-1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7D8636-8B1D-42C9-8C41-99D4332B48B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032AD258-9E86-44FF-8320-6DCB2DCBBB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="153">
   <si>
     <t>Key</t>
   </si>
@@ -262,23 +262,230 @@
     <t>Password:</t>
   </si>
   <si>
-    <t>surname:</t>
-  </si>
-  <si>
     <t>ENG BASE</t>
   </si>
   <si>
     <t>JAPANESE</t>
   </si>
   <si>
-    <t>ARABIC</t>
+    <t>PERSIAN</t>
+  </si>
+  <si>
+    <t>نام کاربری</t>
+  </si>
+  <si>
+    <t>رمز عبور</t>
+  </si>
+  <si>
+    <t>وارد شوید</t>
+  </si>
+  <si>
+    <t>هنوز کاربر نیستید؟</t>
+  </si>
+  <si>
+    <t>یک کاربر جدید ایجاد کنید!</t>
+  </si>
+  <si>
+    <t>به SHOUT! بپیوندید</t>
+  </si>
+  <si>
+    <t>نام کوچک:</t>
+  </si>
+  <si>
+    <t>نام خانوادگی:</t>
+  </si>
+  <si>
+    <t>ایمیل:</t>
+  </si>
+  <si>
+    <t>تاریخ تولد: (روز.ماه.سال)</t>
+  </si>
+  <si>
+    <t>تاریخ تولد خود را انتخاب کنید…</t>
+  </si>
+  <si>
+    <t>نام کاربری:</t>
+  </si>
+  <si>
+    <t>رمز عبور:</t>
+  </si>
+  <si>
+    <t>رمز عبور مجدد:</t>
+  </si>
+  <si>
+    <t>برگشت</t>
+  </si>
+  <si>
+    <t>ثبت نام کنید</t>
+  </si>
+  <si>
+    <t>اضافه کردن پست</t>
+  </si>
+  <si>
+    <t>خوراک</t>
+  </si>
+  <si>
+    <t>نمایه</t>
+  </si>
+  <si>
+    <t>جستجو برای دوستان</t>
+  </si>
+  <si>
+    <t>دوست دارد</t>
+  </si>
+  <si>
+    <t>مانند</t>
+  </si>
+  <si>
+    <t>نظرات</t>
+  </si>
+  <si>
+    <t>نظر دهید</t>
+  </si>
+  <si>
+    <t>کامنت بنویس…</t>
+  </si>
+  <si>
+    <t>حذف کنید</t>
+  </si>
+  <si>
+    <t>لغو کنید</t>
+  </si>
+  <si>
+    <t>امروز به چی فکر می‌کنی؟</t>
+  </si>
+  <si>
+    <t>دوستان</t>
+  </si>
+  <si>
+    <t>تغییر اطلاعات</t>
+  </si>
+  <si>
+    <t>نام:</t>
+  </si>
+  <si>
+    <t>تولد:</t>
+  </si>
+  <si>
+    <t>تغییر آواتار</t>
+  </si>
+  <si>
+    <t>بازگشت</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>درخواست کنید</t>
+  </si>
+  <si>
+    <t>ユーザー名</t>
+  </si>
+  <si>
+    <t>パスワード</t>
+  </si>
+  <si>
+    <t>ログイン</t>
+  </si>
+  <si>
+    <t>まだユーザーではありませんか?</t>
+  </si>
+  <si>
+    <t>新しいユーザーを作成してください!</t>
+  </si>
+  <si>
+    <t>SHOUTに登録しましょう！</t>
+  </si>
+  <si>
+    <t>ファーストネーム：</t>
+  </si>
+  <si>
+    <t>苗字：</t>
+  </si>
+  <si>
+    <t>電子メール:</t>
+  </si>
+  <si>
+    <t>生年月日: (DD.MM.YYYY)</t>
+  </si>
+  <si>
+    <t>生年月日を選択してください…</t>
+  </si>
+  <si>
+    <t>ユーザー名:</t>
+  </si>
+  <si>
+    <t>パスワード:</t>
+  </si>
+  <si>
+    <t>パスワードをもう一度:</t>
+  </si>
+  <si>
+    <t>戻る</t>
+  </si>
+  <si>
+    <t>登録する</t>
+  </si>
+  <si>
+    <t>投稿を追加</t>
+  </si>
+  <si>
+    <t>食べさせる</t>
+  </si>
+  <si>
+    <t>プロフィール</t>
+  </si>
+  <si>
+    <t>友達を探す</t>
+  </si>
+  <si>
+    <t>いいね！</t>
+  </si>
+  <si>
+    <t>のように</t>
+  </si>
+  <si>
+    <t>コメント</t>
+  </si>
+  <si>
+    <t>コメントを書いて…</t>
+  </si>
+  <si>
+    <t>消す</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
+  <si>
+    <t>今日は何を考えていますか？</t>
+  </si>
+  <si>
+    <t>友達</t>
+  </si>
+  <si>
+    <t>変更情報</t>
+  </si>
+  <si>
+    <t>名前：</t>
+  </si>
+  <si>
+    <t>誕生日：</t>
+  </si>
+  <si>
+    <t>アバターの変更</t>
+  </si>
+  <si>
+    <t>姓：</t>
+  </si>
+  <si>
+    <t>適用する</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +500,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -389,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -398,7 +615,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -430,6 +646,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,27 +958,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -764,9 +987,8 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -774,7 +996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -782,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -790,7 +1012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -798,7 +1020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -806,11 +1028,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -818,7 +1040,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -826,7 +1048,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
@@ -834,7 +1056,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>63</v>
       </c>
@@ -842,7 +1064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -850,7 +1072,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>65</v>
       </c>
@@ -858,7 +1080,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
@@ -866,7 +1088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -874,7 +1096,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
@@ -882,7 +1104,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -890,7 +1112,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -898,11 +1120,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -910,7 +1132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -918,7 +1140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -926,7 +1148,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -934,11 +1156,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -946,7 +1168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -954,7 +1176,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -962,7 +1184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -970,7 +1192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -978,7 +1200,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -986,7 +1208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -994,7 +1216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -1002,7 +1224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
@@ -1010,11 +1232,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1022,7 +1244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1030,7 +1252,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1038,7 +1260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1046,7 +1268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1054,7 +1276,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -1062,11 +1284,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -1074,7 +1296,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -1082,7 +1304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -1090,7 +1312,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1098,7 +1320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1106,7 +1328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1114,855 +1336,1023 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A51" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="101" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A101" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B102" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C102" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+    <row r="103" spans="1:3">
+      <c r="A103" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B103" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="10"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="C103" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B104" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="C104" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B105" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="C105" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B106" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="C106" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B107" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="C107" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B109" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="10"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+      <c r="C109" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B110" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+      <c r="C110" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B111" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="10"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="C111" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B112" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+      <c r="C112" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B113" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="10"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="C113" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B114" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+      <c r="C114" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B115" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C65" s="10"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="C115" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B116" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
+      <c r="C116" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B117" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="10"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
+      <c r="C117" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B118" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="C118" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B119" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C69" s="10"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+      <c r="C119" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B121" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="10"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="C121" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B122" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+      <c r="C122" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B123" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C73" s="10"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+      <c r="C123" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B124" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+      <c r="C124" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B126" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+      <c r="C126" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B127" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C77" s="10"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+      <c r="C127" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B128" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+      <c r="C128" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B129" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C79" s="10"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+      <c r="C129" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B130" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="C130" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B131" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C81" s="10"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
+      <c r="C131" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B132" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
+      <c r="C132" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B133" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C83" s="10"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
+      <c r="C133" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B134" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="s">
+      <c r="C134" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="11"/>
+      <c r="B135" s="11"/>
+      <c r="C135" s="11"/>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B136" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="s">
+      <c r="C136" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B137" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="10"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="10" t="s">
+      <c r="C137" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B138" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
+      <c r="C138" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B139" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C89" s="10"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+      <c r="C139" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B140" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="C140" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B141" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="10"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+      <c r="C141" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C93" s="10"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+      <c r="C143" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B144" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
+      <c r="C144" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B145" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C95" s="10"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
+      <c r="C145" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B146" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
+      <c r="C146" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B147" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="10"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="10" t="s">
+      <c r="C147" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B148" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="s">
+      <c r="C148" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C99" s="10"/>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B102" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="12"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" s="12"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C105" s="12"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B106" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C106" s="12"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B107" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C107" s="12"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
-      <c r="B108" s="12"/>
-      <c r="C108" s="12"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B109" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C109" s="12"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C110" s="12"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="12"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C112" s="12"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C113" s="12"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C114" s="12"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C115" s="12"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B116" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C116" s="12"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C117" s="12"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C118" s="12"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C119" s="12"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="12"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B121" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C121" s="12"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C122" s="12"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B123" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C123" s="12"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B124" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C124" s="12"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B126" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C126" s="12"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B127" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="12"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B128" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C128" s="12"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B129" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C129" s="12"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C130" s="12"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B131" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C131" s="12"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B132" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C132" s="12"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B133" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C133" s="12"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B134" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C134" s="12"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="12"/>
-      <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B136" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C136" s="12"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B137" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C137" s="12"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C138" s="12"/>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B139" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C139" s="12"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B140" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C140" s="12"/>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B141" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C141" s="12"/>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
-      <c r="C142" s="12"/>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B143" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C143" s="12"/>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B144" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C144" s="12"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B145" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C145" s="12"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B146" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C146" s="12"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B147" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C147" s="12"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B148" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C148" s="12"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B149" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C149" s="12"/>
+      <c r="B149" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C149" s="16" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add error messages and success prompts for all three languages
</commit_message>
<xml_diff>
--- a/documents/translations.xlsx
+++ b/documents/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\IdeaProjects\OTP-1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032AD258-9E86-44FF-8320-6DCB2DCBBB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4090D3-89CE-484F-8EBC-6A1932418BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="240" windowWidth="15375" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="174">
   <si>
     <t>Key</t>
   </si>
@@ -479,6 +479,69 @@
   </si>
   <si>
     <t>適用する</t>
+  </si>
+  <si>
+    <t>login.fillfields</t>
+  </si>
+  <si>
+    <t>login.incorrectinfo</t>
+  </si>
+  <si>
+    <t>Please fill in all fields</t>
+  </si>
+  <si>
+    <t>User not found</t>
+  </si>
+  <si>
+    <t>register.successfulprompt</t>
+  </si>
+  <si>
+    <t>login.succesfulprompt</t>
+  </si>
+  <si>
+    <t>register.fillfields</t>
+  </si>
+  <si>
+    <t>User registered succesfully</t>
+  </si>
+  <si>
+    <t>register.emailtaken</t>
+  </si>
+  <si>
+    <t>Email already taken</t>
+  </si>
+  <si>
+    <t>User logged in succesfully</t>
+  </si>
+  <si>
+    <t>すべての項目にご記入ください</t>
+  </si>
+  <si>
+    <t>ユーザー登録が完了しました</t>
+  </si>
+  <si>
+    <t>メールはすでに受信されています</t>
+  </si>
+  <si>
+    <t>ユーザーが見つかりません</t>
+  </si>
+  <si>
+    <t>ユーザーは正常にログインしました</t>
+  </si>
+  <si>
+    <t>کاربر با موفقیت وارد سیستم شد</t>
+  </si>
+  <si>
+    <t>کاربر پیدا نشد</t>
+  </si>
+  <si>
+    <t>لطفا همه فیلدها را پر کنید</t>
+  </si>
+  <si>
+    <t>کاربر با موفقیت ثبت نام کرد</t>
+  </si>
+  <si>
+    <t>ایمیل قبلاً گرفته شده است</t>
   </si>
 </sst>
 </file>
@@ -958,17 +1021,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1029,517 +1092,484 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>16</v>
+        <v>157</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A51" s="6" t="s">
+    <row r="59" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A60" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="7" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="9" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="9" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="9" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="9" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="9" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="9" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="9" t="s">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="9" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1549,812 +1579,1048 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="9" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="9" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="9" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="9" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="9"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
+      <c r="A75" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="9" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="9" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="9" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="9" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="9" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="9" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="9" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="9" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="9" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>24</v>
+        <v>162</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
+      <c r="C85" s="18"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>146</v>
-      </c>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="9" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="9" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="9" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="9" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C91" s="18" t="s">
-        <v>149</v>
-      </c>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
+      <c r="A92" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="9" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="9" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="9" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="9" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="9" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="9" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B115" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C99" s="18" t="s">
+      <c r="C115" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A101" s="10" t="s">
+    <row r="116" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="117" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A117" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="12" t="s">
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B118" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C118" s="14" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C105" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C106" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C107" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C109" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C110" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C112" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C113" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C114" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C115" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C116" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C117" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C118" s="16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="11" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
+      <c r="A120" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="11" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="11"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
+      <c r="A125" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C125" s="16" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="11" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>103</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="16" t="s">
-        <v>104</v>
-      </c>
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="16"/>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C128" s="16" t="s">
-        <v>105</v>
-      </c>
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="11" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C129" s="16" t="s">
-        <v>106</v>
+        <v>70</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="11" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="11" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="11" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="11" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11"/>
-      <c r="C135" s="11"/>
+      <c r="A135" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="11" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="11" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="11" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="11" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="11" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>48</v>
+        <v>155</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="11" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>114</v>
+        <v>172</v>
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="11"/>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
+      <c r="A142" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C142" s="16" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B143" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>115</v>
-      </c>
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="11" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C144" s="16" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="11" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="11" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="11" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B148" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C148" s="16" t="s">
-        <v>116</v>
-      </c>
+      <c r="A148" s="11"/>
+      <c r="B148" s="11"/>
+      <c r="C148" s="11"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B152" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B153" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C153" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C154" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C156" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="11"/>
+      <c r="B158" s="11"/>
+      <c r="C158" s="11"/>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C159" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B160" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C160" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C162" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B164" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C164" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="11"/>
+      <c r="B165" s="11"/>
+      <c r="C165" s="11"/>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C166" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C167" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C168" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C169" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B170" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C170" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C171" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B149" s="11" t="s">
+      <c r="B172" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C149" s="16" t="s">
+      <c r="C172" s="16" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delete extra empty rows
</commit_message>
<xml_diff>
--- a/documents/translations.xlsx
+++ b/documents/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\IdeaProjects\OTP-1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4090D3-89CE-484F-8EBC-6A1932418BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E8636-AEF5-4471-8754-0BBEA3A9D771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="240" windowWidth="15375" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1021,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,1386 +1236,1369 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>57</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A57" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A60" s="6" t="s">
-        <v>81</v>
+      <c r="A58" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>2</v>
+      <c r="A61" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="9" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="9" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="9" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>12</v>
+        <v>163</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>164</v>
-      </c>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="9" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="9" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
+      <c r="A70" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="9" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="9" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="9" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="9" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>77</v>
+        <v>160</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="9" t="s">
-        <v>75</v>
+        <v>161</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>164</v>
-      </c>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="9" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="9" t="s">
-        <v>161</v>
+        <v>14</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="18"/>
+      <c r="A85" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C87" s="18" t="s">
-        <v>135</v>
-      </c>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
+      <c r="A91" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>143</v>
-      </c>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="9" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="9" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
+      <c r="A101" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>148</v>
-      </c>
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="9"/>
-      <c r="B108" s="9"/>
-      <c r="C108" s="9"/>
+      <c r="A108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C112" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C113" s="18" t="s">
-        <v>149</v>
-      </c>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="113" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A113" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C114" s="18" t="s">
-        <v>133</v>
+      <c r="A114" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C115" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A117" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
+      <c r="A115" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>2</v>
+      <c r="A118" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="11" t="s">
-        <v>4</v>
+        <v>153</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>84</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="11" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="11" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B123" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C123" s="16" t="s">
-        <v>87</v>
-      </c>
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="16"/>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B124" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C124" s="16" t="s">
-        <v>171</v>
-      </c>
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="11" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C125" s="16" t="s">
-        <v>170</v>
+        <v>70</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="11" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="11"/>
-      <c r="B127" s="11"/>
-      <c r="C127" s="16"/>
+      <c r="A127" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
+      <c r="A128" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="11" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C129" s="17" t="s">
-        <v>88</v>
+        <v>67</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="11" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="11" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="11" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="11" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="11" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="11" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B139" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C139" s="16" t="s">
-        <v>98</v>
-      </c>
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
+      <c r="C139" s="11"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="11" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="11" t="s">
-        <v>157</v>
+        <v>14</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="11" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>173</v>
+        <v>101</v>
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="11"/>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
+      <c r="A143" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B144" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C144" s="16" t="s">
-        <v>99</v>
-      </c>
+      <c r="A144" s="11"/>
+      <c r="B144" s="11"/>
+      <c r="C144" s="11"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
+      <c r="A148" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B148" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C148" s="16" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B154" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C154" s="16" t="s">
-        <v>108</v>
-      </c>
+      <c r="A154" s="11"/>
+      <c r="B154" s="11"/>
+      <c r="C154" s="11"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="11" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B155" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="11" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B156" s="11" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="11" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="11"/>
-      <c r="B158" s="11"/>
-      <c r="C158" s="11"/>
+      <c r="A158" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="11" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B159" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B160" s="11" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C161" s="16" t="s">
-        <v>113</v>
-      </c>
+      <c r="A161" s="11"/>
+      <c r="B161" s="11"/>
+      <c r="C161" s="11"/>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="11"/>
-      <c r="B165" s="11"/>
-      <c r="C165" s="11"/>
+      <c r="A165" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B165" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C165" s="16" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B168" s="11" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C168" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C169" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B170" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C170" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B171" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C171" s="16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C172" s="16" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>